<commit_message>
Xiling's diary updated Jan 22.
</commit_message>
<xml_diff>
--- a/diaries/diary-xiling-li.xlsx
+++ b/diaries/diary-xiling-li.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lixiling/Documents/UCI/courses/265p/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B910B3-F555-9A4A-B5AC-BC1B98A56402}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230F6064-9E18-C14A-9740-12812AE68104}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="6040" windowWidth="29040" windowHeight="17800" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="3900" yWindow="2760" windowWidth="28060" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -48,39 +48,18 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
     <t>Etc.</t>
   </si>
   <si>
@@ -109,6 +88,36 @@
   </si>
   <si>
     <t>https://github.com/xilingl1/</t>
+  </si>
+  <si>
+    <t>Jan 16 2020</t>
+  </si>
+  <si>
+    <t>Learn about code reading strategy</t>
+  </si>
+  <si>
+    <t>Learned different styles and discovered my own preference</t>
+  </si>
+  <si>
+    <t>Listening to other students' reading strategy surprised me, because it is so different from me. I thought, 'Very organised thinking, but why bother that much of rest of the code?' Then I am happy I volunteered to try reading code during class. Because of that my learning experience enhanced. Thinking out loud made me realized clearly what my reading strategy is, and the benefit of other's strategy. And I enjoyed the guest talk. Made me realize that I should do more research into the industry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I enjoyed it all the way, I cannot thinking  of ditching any part of the class. </t>
+  </si>
+  <si>
+    <t>Jan 21 2020</t>
+  </si>
+  <si>
+    <t>frustrated -&gt; pull myself  up again -&gt; still a little confused, but encouraged</t>
+  </si>
+  <si>
+    <t>Homework &amp; Pull Request</t>
+  </si>
+  <si>
+    <t>Both done.</t>
+  </si>
+  <si>
+    <t>I spend almost whole day trying to finish all the homework. Reading code is still not easy to me. During the code reading I gradually refined my reading strategy, I lowered my intent to do opportunistic comprehension and do more systematic comprehension. I think things work out better. After created a wrong pull request I spent some time learning more about Git &amp; Github. I found a video on youtube which is quite helpful.</t>
   </si>
 </sst>
 </file>
@@ -602,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F15" sqref="F14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -658,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -671,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -708,90 +717,86 @@
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" s="10">
         <v>0.95833333333333337</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="7" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="B12" s="10">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>

</xml_diff>